<commit_message>
add google drive snapshot from end of week4
</commit_message>
<xml_diff>
--- a/google-drive/client/client-questions.xlsx
+++ b/google-drive/client/client-questions.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mh370DMJoM/MpCl7Ti3DJrDW/9/QQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miIffUcP2VG2arJLjlUGe4n5OmTbg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t>Asked</t>
   </si>
@@ -78,6 +78,9 @@
     <t>What is the range of time that bays can be reserved? 9-5pm?</t>
   </si>
   <si>
+    <t>9-5, business days</t>
+  </si>
+  <si>
     <t>People who can book a bay</t>
   </si>
   <si>
@@ -123,6 +126,9 @@
     <t>List will be preffered (keep it simple)</t>
   </si>
   <si>
+    <t>Can we change the colour code of the system to match the library one? e.g. Green = available, Red = taken, Yellow = layover period</t>
+  </si>
+  <si>
     <t>Approval</t>
   </si>
   <si>
@@ -162,6 +168,12 @@
     <t>If so, would what contact info would you want from user? email, mobile, name?</t>
   </si>
   <si>
+    <t>like library but choose multiple - mentioned contact below</t>
+  </si>
+  <si>
+    <t>Have you decided if you would like the option for the T&amp;C tick box (may need to come back to it later)</t>
+  </si>
+  <si>
     <t>A3 Reservation sign</t>
   </si>
   <si>
@@ -174,6 +186,9 @@
     <t>Do you want an email sent early morning with all A3 reservation signs or as the booking is made?</t>
   </si>
   <si>
+    <t>separate for each email, name rego times date (name more important than rego) date time to - not required rego</t>
+  </si>
+  <si>
     <t>I would say they want it early morning the day of so we can put multiple bookings onto one sheet (save paper)</t>
   </si>
   <si>
@@ -198,6 +213,9 @@
     <t>Maybe have a map that can guide users to the bay</t>
   </si>
   <si>
+    <t>Single page web app functionality as extension?</t>
+  </si>
+  <si>
     <t>Appearance</t>
   </si>
   <si>
@@ -205,6 +223,9 @@
   </si>
   <si>
     <t>Can you provide us with the graphics, fonts you previously mentioned?</t>
+  </si>
+  <si>
+    <t>yes, will send to us</t>
   </si>
   <si>
     <t>Other</t>
@@ -229,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -271,14 +292,14 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Docs-calibri"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -291,18 +312,18 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="10.0"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FFFF00FF"/>
+      <i/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -356,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -377,24 +398,19 @@
     <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="6" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -613,9 +629,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.14"/>
-    <col customWidth="1" min="2" max="2" width="71.14"/>
+    <col customWidth="1" min="2" max="2" width="167.57"/>
     <col customWidth="1" min="3" max="3" width="154.43"/>
-    <col customWidth="1" min="4" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="30.75" customHeight="1">
@@ -734,7 +749,9 @@
       <c r="B16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -747,16 +764,16 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -770,26 +787,26 @@
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -805,39 +822,42 @@
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="13"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
@@ -849,39 +869,39 @@
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="5"/>
       <c r="B45" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="14"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" ht="15.75" customHeight="1"/>
     <row r="48" ht="15.75" customHeight="1"/>
@@ -893,50 +913,60 @@
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C50" s="3"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="5"/>
       <c r="B51" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="5"/>
       <c r="B52" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="15"/>
-      <c r="B53" s="16" t="s">
-        <v>45</v>
+      <c r="A53" s="16"/>
+      <c r="B53" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C53" s="10"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="15"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C54" s="17"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="18"/>
-      <c r="B55" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C55" s="17"/>
-    </row>
-    <row r="56" ht="15.75" customHeight="1"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="9"/>
+      <c r="B56" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="18" t="str">
+        <f>ARRAY_CONSTRAIN(ARRAYFORMULA(- generic tick to accept), 1, 1)</f>
+        <v>#ERROR!</v>
+      </c>
+    </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1">
@@ -947,26 +977,29 @@
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C60" s="3"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="5"/>
       <c r="B61" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="9"/>
       <c r="B62" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1"/>
@@ -980,126 +1013,137 @@
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="5"/>
       <c r="B68" s="6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="5"/>
       <c r="B69" s="6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="5"/>
       <c r="B70" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="14"/>
+      <c r="A71" s="20"/>
+      <c r="B71" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" s="15"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="14"/>
+      <c r="A72" s="21"/>
+      <c r="C72" s="15"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="14"/>
+      <c r="C73" s="15"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
+      <c r="C74" s="15"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="3"/>
-      <c r="B75" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="B75" s="3"/>
       <c r="C75" s="3"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="5"/>
-      <c r="B76" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="A76" s="3"/>
+      <c r="B76" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C76" s="3"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="9"/>
-      <c r="B77" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C77" s="17"/>
-    </row>
-    <row r="78" ht="15.75" customHeight="1"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="9"/>
+      <c r="B78" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="79" ht="15.75" customHeight="1"/>
     <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-    </row>
+    <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="3"/>
-      <c r="B82" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="B82" s="3"/>
       <c r="C82" s="3"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="5"/>
-      <c r="B83" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="A83" s="3"/>
+      <c r="B83" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="18"/>
-      <c r="B84" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>67</v>
+      <c r="A84" s="5"/>
+      <c r="B84" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="18"/>
-      <c r="B85" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="9"/>
+      <c r="B86" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="A87" s="22"/>
+    </row>
     <row r="88" ht="15.75" customHeight="1"/>
     <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-    </row>
-    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+    </row>
     <row r="92" ht="15.75" customHeight="1"/>
     <row r="93" ht="15.75" customHeight="1"/>
     <row r="94" ht="15.75" customHeight="1"/>
@@ -2014,6 +2058,7 @@
     <row r="1003" ht="15.75" customHeight="1"/>
     <row r="1004" ht="15.75" customHeight="1"/>
     <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>